<commit_message>
add day class subject
</commit_message>
<xml_diff>
--- a/public/file/excel/excel-students.xlsx
+++ b/public/file/excel/excel-students.xlsx
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
fix views, add count study, add dash
</commit_message>
<xml_diff>
--- a/public/file/excel/excel-students.xlsx
+++ b/public/file/excel/excel-students.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="53">
   <si>
     <t>Full name</t>
   </si>
@@ -69,51 +69,6 @@
     <t>0902313145</t>
   </si>
   <si>
-    <t>Long Tran</t>
-  </si>
-  <si>
-    <t>Cuc thi</t>
-  </si>
-  <si>
-    <t>Hoang Khang</t>
-  </si>
-  <si>
-    <t>Khong Tu Quynh</t>
-  </si>
-  <si>
-    <t>Diep Van</t>
-  </si>
-  <si>
-    <t>Ga Lét Beo</t>
-  </si>
-  <si>
-    <t>Thu Đi ĐI</t>
-  </si>
-  <si>
-    <t>Xuân Đến Rồi</t>
-  </si>
-  <si>
-    <t>Hè Ấm Áp</t>
-  </si>
-  <si>
-    <t>Vui vẻ Hông Quạo</t>
-  </si>
-  <si>
-    <t>Gao Đen</t>
-  </si>
-  <si>
-    <t>Gao Đỏ</t>
-  </si>
-  <si>
-    <t>Gao Vàng</t>
-  </si>
-  <si>
-    <t>Gao Heo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gao dog </t>
-  </si>
-  <si>
     <t>MSSV</t>
   </si>
   <si>
@@ -126,52 +81,100 @@
     <t xml:space="preserve">Class code </t>
   </si>
   <si>
-    <t>ps09110</t>
-  </si>
-  <si>
-    <t>ps09111</t>
-  </si>
-  <si>
-    <t>ps09112</t>
-  </si>
-  <si>
-    <t>ps09113</t>
-  </si>
-  <si>
-    <t>ps09114</t>
-  </si>
-  <si>
-    <t>ps09115</t>
-  </si>
-  <si>
-    <t>ps09116</t>
-  </si>
-  <si>
-    <t>ps09117</t>
-  </si>
-  <si>
-    <t>ps09118</t>
-  </si>
-  <si>
-    <t>ps09119</t>
-  </si>
-  <si>
-    <t>ps09120</t>
-  </si>
-  <si>
-    <t>ps09121</t>
-  </si>
-  <si>
-    <t>ps09122</t>
-  </si>
-  <si>
-    <t>ps09123</t>
-  </si>
-  <si>
-    <t>ps09124</t>
-  </si>
-  <si>
-    <t>WD14301</t>
+    <t>ps09125</t>
+  </si>
+  <si>
+    <t>ps09126</t>
+  </si>
+  <si>
+    <t>ps09127</t>
+  </si>
+  <si>
+    <t>ps09128</t>
+  </si>
+  <si>
+    <t>ps09129</t>
+  </si>
+  <si>
+    <t>ps09130</t>
+  </si>
+  <si>
+    <t>ps09131</t>
+  </si>
+  <si>
+    <t>ps09132</t>
+  </si>
+  <si>
+    <t>ps09133</t>
+  </si>
+  <si>
+    <t>ps09134</t>
+  </si>
+  <si>
+    <t>ps09135</t>
+  </si>
+  <si>
+    <t>ps09136</t>
+  </si>
+  <si>
+    <t>ps09137</t>
+  </si>
+  <si>
+    <t>ps09138</t>
+  </si>
+  <si>
+    <t>ps09139</t>
+  </si>
+  <si>
+    <t>Đen Vâu</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Phương Mỹ Chi</t>
+  </si>
+  <si>
+    <t>Khoa Phạm</t>
+  </si>
+  <si>
+    <t>Code X</t>
+  </si>
+  <si>
+    <t>Điệp Vấn 2</t>
+  </si>
+  <si>
+    <t>Rô nal đô</t>
+  </si>
+  <si>
+    <t>Tiki Nguyễn</t>
+  </si>
+  <si>
+    <t>Ô Lông Nguyễn</t>
+  </si>
+  <si>
+    <t>Heo Xinh Trần</t>
+  </si>
+  <si>
+    <t>Hà Anh Tuấn</t>
+  </si>
+  <si>
+    <t>Sơn Tùng</t>
+  </si>
+  <si>
+    <t>What đờ phắc</t>
+  </si>
+  <si>
+    <t>Ta đa nguyễn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mèo ú </t>
+  </si>
+  <si>
+    <t>Mèo mướp</t>
+  </si>
+  <si>
+    <t>WD14306</t>
   </si>
 </sst>
 </file>
@@ -522,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -536,29 +539,29 @@
     <col min="5" max="5" width="12.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
         <v>36</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
@@ -567,15 +570,15 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
@@ -584,15 +587,15 @@
         <v>1</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>4</v>
@@ -601,15 +604,15 @@
         <v>1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>5</v>
@@ -618,15 +621,15 @@
         <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>6</v>
@@ -635,15 +638,15 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>7</v>
@@ -652,15 +655,15 @@
         <v>1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>8</v>
@@ -669,15 +672,15 @@
         <v>1</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>9</v>
@@ -686,15 +689,15 @@
         <v>1</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>10</v>
@@ -703,15 +706,18 @@
         <v>1</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+      <c r="I10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>11</v>
@@ -720,15 +726,15 @@
         <v>1</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>12</v>
@@ -737,15 +743,15 @@
         <v>1</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>13</v>
@@ -754,15 +760,15 @@
         <v>1</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>14</v>
@@ -771,15 +777,15 @@
         <v>1</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>15</v>
@@ -788,15 +794,15 @@
         <v>1</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>16</v>
@@ -805,7 +811,7 @@
         <v>1</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>